<commit_message>
change data directory names.
</commit_message>
<xml_diff>
--- a/park_lookup.xlsx
+++ b/park_lookup.xlsx
@@ -3261,7 +3261,11 @@
           <t>Civil War Defenses of Washington</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr"/>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Park</t>
+        </is>
+      </c>
       <c r="D105" t="inlineStr">
         <is>
           <t>DC,MD,VA</t>
@@ -7077,7 +7081,11 @@
           <t>I&amp;#241;upiat Heritage Center</t>
         </is>
       </c>
-      <c r="C242" t="inlineStr"/>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Heritage Center</t>
+        </is>
+      </c>
       <c r="D242" t="inlineStr">
         <is>
           <t>AK</t>

</xml_diff>